<commit_message>
Day-12 Notes and examples
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\JAVA Fsd 12th April Batch 7 30 Am\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java Fsd 12th April Batch 7 30 PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7252271-DE45-4768-80C9-F740926EB792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E31A1B-1A8C-4463-82BA-DDF1C604F927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Concepts</t>
   </si>
@@ -88,76 +88,115 @@
     <t>Day-1</t>
   </si>
   <si>
-    <t>Day-39</t>
-  </si>
-  <si>
-    <t>Day-40</t>
-  </si>
-  <si>
-    <t>Day-41</t>
-  </si>
-  <si>
-    <t>Day-42</t>
-  </si>
-  <si>
-    <t>Day-43</t>
-  </si>
-  <si>
-    <t>JS</t>
-  </si>
-  <si>
-    <t>TS</t>
-  </si>
-  <si>
-    <t>Validations and exception handling for case study and JPA and CRUD repository</t>
-  </si>
-  <si>
-    <t>7:40AM-8:36AM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Revise The Basic Version history features of java </t>
   </si>
   <si>
-    <t>https://github.com/sandeepsomavarapu/OnlineTraining9_april_2023-7-30AM.git</t>
-  </si>
-  <si>
-    <t xml:space="preserve">download and install java and eclipse </t>
+    <t>8:10PM -9:00PM</t>
   </si>
   <si>
     <t>Day-2</t>
   </si>
   <si>
-    <t>7:40AM-8:50AM</t>
-  </si>
-  <si>
-    <t>https://www.eclipse.org/downloads/packages/release/2020-12/r</t>
+    <t>java execution flow,jdk,jvm,jre</t>
+  </si>
+  <si>
+    <t>7:30pm-8:25PM</t>
+  </si>
+  <si>
+    <t>complete the eclipse and java installation</t>
+  </si>
+  <si>
+    <t>https://www.javatpoint.com/javafx-how-to-install-java</t>
   </si>
   <si>
     <t>Day-3</t>
   </si>
   <si>
-    <t>compailation,execution flow,java setup,.java,.class,compiler,jvm</t>
-  </si>
-  <si>
     <t>identifiers,variables,datatypes</t>
   </si>
   <si>
-    <t>7:30AM-8:55AM</t>
-  </si>
-  <si>
-    <t>download and install java and eclipse and revise variables  and keywords,language fundamentals notes</t>
+    <t>revise the concepts</t>
   </si>
   <si>
     <t>Day-4</t>
   </si>
   <si>
-    <t>instance.static variables ,ECLIPSE</t>
-  </si>
-  <si>
-    <t>7:35AM-8:35AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revise instance and static </t>
+    <t>instance,static  variables &amp;Eclipse</t>
+  </si>
+  <si>
+    <t>7:45PM-8:30PM</t>
+  </si>
+  <si>
+    <t>Day-5</t>
+  </si>
+  <si>
+    <t>7:35 PM-8:28PM</t>
+  </si>
+  <si>
+    <t>Methods,flow control</t>
+  </si>
+  <si>
+    <t>Complete the assignment on flow control</t>
+  </si>
+  <si>
+    <t>Day-6</t>
+  </si>
+  <si>
+    <t>OOPS</t>
+  </si>
+  <si>
+    <t>Day-7</t>
+  </si>
+  <si>
+    <t>7:40 PM-8:28PM</t>
+  </si>
+  <si>
+    <t>OOPS,inheritance,class,abstract,interface and concrete and abstract methods</t>
+  </si>
+  <si>
+    <t>Day-8</t>
+  </si>
+  <si>
+    <t>Multiple inheritance,polymorphisam,package,import</t>
+  </si>
+  <si>
+    <t>Day-9</t>
+  </si>
+  <si>
+    <t>method overriding,final,access modifiers</t>
+  </si>
+  <si>
+    <t>Day-10</t>
+  </si>
+  <si>
+    <t>7:50PM-8:30PM</t>
+  </si>
+  <si>
+    <t>Scanner,dynamic input,encapsulation</t>
+  </si>
+  <si>
+    <t>Day-11</t>
+  </si>
+  <si>
+    <t>7:38PM-8:30PM</t>
+  </si>
+  <si>
+    <t>String,Stringbuilder,StringBuffer,JVM Architecutre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String class methods  </t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/java/java_ref_string.asp</t>
+  </si>
+  <si>
+    <t>Day-12</t>
+  </si>
+  <si>
+    <t>Exception Handling</t>
+  </si>
+  <si>
+    <t>Day-13</t>
   </si>
 </sst>
 </file>
@@ -336,7 +375,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -620,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +668,7 @@
     <col min="3" max="3" width="6.21875" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="71.88671875" customWidth="1"/>
+    <col min="6" max="6" width="79.6640625" customWidth="1"/>
     <col min="7" max="7" width="30.109375" customWidth="1"/>
     <col min="8" max="8" width="71.109375" customWidth="1"/>
     <col min="9" max="9" width="68.109375" customWidth="1"/>
@@ -637,9 +676,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F3" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="F3" s="14"/>
       <c r="H3" t="s">
         <v>17</v>
       </c>
@@ -676,10 +713,10 @@
         <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>16</v>
@@ -687,127 +724,197 @@
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4">
         <v>45029</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4">
         <v>45030</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D8" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E8" s="4">
+        <v>45034</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="4">
         <v>45035</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="I9" s="9"/>
     </row>
     <row r="10" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="6"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="D10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4">
+        <v>45036</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="D11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="4">
+        <v>45406</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="D12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="4">
+        <v>45042</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="9"/>
     </row>
     <row r="13" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="D13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="4">
+        <v>45043</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="D14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="4">
+        <v>45044</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D15" s="6"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="D15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="4">
+        <v>45047</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3"/>
+      <c r="D16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="4">
+        <v>45048</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D17" s="6"/>
-      <c r="E17" s="4"/>
+      <c r="D17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="4">
+        <v>45049</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="5"/>
       <c r="H17" s="3"/>
@@ -1021,51 +1128,31 @@
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D43" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="4">
-        <v>45028</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="3"/>
       <c r="G43" s="10"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D44" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="4">
-        <v>45029</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="3"/>
       <c r="G44" s="10"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D45" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="4">
-        <v>45030</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="3"/>
       <c r="G45" s="10"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D46" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -1073,9 +1160,7 @@
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D47" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="D47" s="6"/>
       <c r="E47" s="6"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -1963,11 +2048,10 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I5" r:id="rId1" xr:uid="{C438D4D9-FF94-4163-9A83-2CC81A380B4A}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{55425D7C-77A7-40EC-BE6F-7638B8408219}"/>
-    <hyperlink ref="I6" r:id="rId3" xr:uid="{8F288ACE-2B75-48BA-B846-60D1B8B31F82}"/>
+    <hyperlink ref="I15" r:id="rId2" xr:uid="{FDA3DF84-EEAE-4FFB-ACE6-082120202474}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Day-13 notes and examples
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java Fsd 12th April Batch 7 30 PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E31A1B-1A8C-4463-82BA-DDF1C604F927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D1D238-772B-49BB-B90D-2B6933AAE1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Concepts</t>
   </si>
@@ -197,6 +197,33 @@
   </si>
   <si>
     <t>Day-13</t>
+  </si>
+  <si>
+    <t>Day-14</t>
+  </si>
+  <si>
+    <t>Day-15</t>
+  </si>
+  <si>
+    <t>Day-16</t>
+  </si>
+  <si>
+    <t>Day-17</t>
+  </si>
+  <si>
+    <t>Day-18</t>
+  </si>
+  <si>
+    <t>Day-19</t>
+  </si>
+  <si>
+    <t>Day-20</t>
+  </si>
+  <si>
+    <t>7:30PM-8:30PM</t>
+  </si>
+  <si>
+    <t>take username and password   like    "onlinetraining9" "india" if not throw exception</t>
   </si>
 </sst>
 </file>
@@ -659,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,7 +931,9 @@
       <c r="F16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
@@ -915,13 +944,21 @@
       <c r="E17" s="4">
         <v>45049</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="11"/>
       <c r="G18" s="5"/>
@@ -930,7 +967,9 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
       <c r="G19" s="5"/>
@@ -938,7 +977,9 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
       <c r="G20" s="5"/>
@@ -946,7 +987,9 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3"/>
       <c r="G21" s="5"/>
@@ -954,7 +997,9 @@
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3"/>
       <c r="G22" s="5"/>
@@ -962,7 +1007,9 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D23" s="6"/>
+      <c r="D23" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3"/>
       <c r="G23" s="5"/>
@@ -970,7 +1017,9 @@
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3"/>
       <c r="G24" s="5"/>

</xml_diff>

<commit_message>
Day-16 notes and examples
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java Fsd 12th April Batch 7 30 PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FDE2F3-BA44-41FA-8BE1-D7BF2E0B4763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8C2F07-EE8C-4653-BE6F-8EF860EBF98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>Concepts</t>
   </si>
@@ -681,7 +681,7 @@
   <dimension ref="A3:M171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,9 +988,15 @@
       <c r="D20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="5"/>
+      <c r="E20" s="4">
+        <v>45061</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>

</xml_diff>

<commit_message>
Day-30 Spring boot with case study
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java Fsd 12th April Batch 7 30 PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EB4332-BD76-4D11-95FE-0EB4C138BD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB289C0-D6FB-4DD7-901D-5BE429994653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t>Concepts</t>
   </si>
@@ -265,13 +265,34 @@
     <t xml:space="preserve">JPQL,Persistence life cycle </t>
   </si>
   <si>
-    <t xml:space="preserve">spring </t>
-  </si>
-  <si>
-    <t>spring mvc</t>
-  </si>
-  <si>
     <t>spring boot</t>
+  </si>
+  <si>
+    <t>Day-21</t>
+  </si>
+  <si>
+    <t>Day-22</t>
+  </si>
+  <si>
+    <t>Day-23</t>
+  </si>
+  <si>
+    <t>Day-24</t>
+  </si>
+  <si>
+    <t>Day-25</t>
+  </si>
+  <si>
+    <t>Day-26</t>
+  </si>
+  <si>
+    <t>Day-27</t>
+  </si>
+  <si>
+    <t>spring  framework</t>
+  </si>
+  <si>
+    <t>spring mvc,Spring jpa</t>
   </si>
 </sst>
 </file>
@@ -723,7 +744,7 @@
   <dimension ref="A3:M171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F5" sqref="F5:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,7 +1135,9 @@
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="E25" s="4">
         <v>45070</v>
       </c>
@@ -1129,7 +1152,9 @@
       <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D26" s="6"/>
+      <c r="D26" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="E26" s="4">
         <v>45071</v>
       </c>
@@ -1144,7 +1169,9 @@
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="E27" s="4">
         <v>45076</v>
       </c>
@@ -1158,50 +1185,66 @@
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="E28" s="4">
         <v>45077</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="E29" s="4">
-        <v>45078</v>
+        <v>45083</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>88</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="E30" s="4">
-        <v>45079</v>
+        <v>45084</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G30" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="E31" s="4">
-        <v>45080</v>
+        <v>45085</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>

</xml_diff>